<commit_message>
updat import excel mahasiswa
</commit_message>
<xml_diff>
--- a/public/template_mahasiswa.xlsx
+++ b/public/template_mahasiswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\PBL4_Sem4\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB7C6B3-0A58-4D87-8D28-E390230FB853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9E2FB1-64A4-4D94-8F30-AAE4485EC1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0EAF9244-301C-410D-B4A0-AE62B17C945B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="208">
   <si>
     <t>username</t>
   </si>
@@ -643,6 +643,21 @@
   </si>
   <si>
     <t>+62-0661-185-5886</t>
+  </si>
+  <si>
+    <t>angkatan</t>
+  </si>
+  <si>
+    <t>jenis_kelamin</t>
+  </si>
+  <si>
+    <t>ipk</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -686,9 +701,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28F0C26-52C3-4B30-824C-C017CAFBEA4C}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="E36" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1018,9 +1034,10 @@
     <col min="5" max="5" width="20.7265625" customWidth="1"/>
     <col min="6" max="6" width="18.1796875" customWidth="1"/>
     <col min="7" max="7" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,8 +1059,17 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1065,8 +1091,17 @@
       <c r="G2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>2023</v>
+      </c>
+      <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1088,8 +1123,17 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>2023</v>
+      </c>
+      <c r="I3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J3">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1111,8 +1155,17 @@
       <c r="G4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>2023</v>
+      </c>
+      <c r="I4" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1134,8 +1187,17 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>2023</v>
+      </c>
+      <c r="I5" t="s">
+        <v>206</v>
+      </c>
+      <c r="J5">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1157,8 +1219,17 @@
       <c r="G6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>2023</v>
+      </c>
+      <c r="I6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J6">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1180,8 +1251,17 @@
       <c r="G7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>2023</v>
+      </c>
+      <c r="I7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1203,8 +1283,17 @@
       <c r="G8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>2023</v>
+      </c>
+      <c r="I8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J8">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1226,8 +1315,17 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>2023</v>
+      </c>
+      <c r="I9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J9">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1249,8 +1347,17 @@
       <c r="G10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>2023</v>
+      </c>
+      <c r="I10" t="s">
+        <v>206</v>
+      </c>
+      <c r="J10">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1272,8 +1379,17 @@
       <c r="G11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>2023</v>
+      </c>
+      <c r="I11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J11">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1295,8 +1411,17 @@
       <c r="G12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>2023</v>
+      </c>
+      <c r="I12" t="s">
+        <v>206</v>
+      </c>
+      <c r="J12">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1318,8 +1443,17 @@
       <c r="G13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>2023</v>
+      </c>
+      <c r="I13" t="s">
+        <v>206</v>
+      </c>
+      <c r="J13">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1341,8 +1475,17 @@
       <c r="G14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>2023</v>
+      </c>
+      <c r="I14" t="s">
+        <v>207</v>
+      </c>
+      <c r="J14">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1364,8 +1507,17 @@
       <c r="G15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>2023</v>
+      </c>
+      <c r="I15" t="s">
+        <v>207</v>
+      </c>
+      <c r="J15">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1387,8 +1539,17 @@
       <c r="G16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>2023</v>
+      </c>
+      <c r="I16" t="s">
+        <v>207</v>
+      </c>
+      <c r="J16" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1410,8 +1571,17 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>2023</v>
+      </c>
+      <c r="I17" t="s">
+        <v>207</v>
+      </c>
+      <c r="J17">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -1433,8 +1603,17 @@
       <c r="G18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>2023</v>
+      </c>
+      <c r="I18" t="s">
+        <v>207</v>
+      </c>
+      <c r="J18">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -1456,8 +1635,17 @@
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>2023</v>
+      </c>
+      <c r="I19" t="s">
+        <v>207</v>
+      </c>
+      <c r="J19" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -1479,8 +1667,17 @@
       <c r="G20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20">
+        <v>2023</v>
+      </c>
+      <c r="I20" t="s">
+        <v>207</v>
+      </c>
+      <c r="J20">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1502,8 +1699,17 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21">
+        <v>2022</v>
+      </c>
+      <c r="I21" t="s">
+        <v>207</v>
+      </c>
+      <c r="J21">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1525,8 +1731,17 @@
       <c r="G22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22">
+        <v>2022</v>
+      </c>
+      <c r="I22" t="s">
+        <v>207</v>
+      </c>
+      <c r="J22">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -1548,8 +1763,17 @@
       <c r="G23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <v>2022</v>
+      </c>
+      <c r="I23" t="s">
+        <v>207</v>
+      </c>
+      <c r="J23">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1571,8 +1795,17 @@
       <c r="G24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <v>2022</v>
+      </c>
+      <c r="I24" t="s">
+        <v>207</v>
+      </c>
+      <c r="J24">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -1594,8 +1827,17 @@
       <c r="G25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25">
+        <v>2022</v>
+      </c>
+      <c r="I25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J25">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -1617,8 +1859,17 @@
       <c r="G26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26">
+        <v>2022</v>
+      </c>
+      <c r="I26" t="s">
+        <v>207</v>
+      </c>
+      <c r="J26">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -1640,8 +1891,17 @@
       <c r="G27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27">
+        <v>2022</v>
+      </c>
+      <c r="I27" t="s">
+        <v>207</v>
+      </c>
+      <c r="J27">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -1663,8 +1923,17 @@
       <c r="G28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28">
+        <v>2022</v>
+      </c>
+      <c r="I28" t="s">
+        <v>207</v>
+      </c>
+      <c r="J28" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -1686,8 +1955,17 @@
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29">
+        <v>2022</v>
+      </c>
+      <c r="I29" t="s">
+        <v>207</v>
+      </c>
+      <c r="J29">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -1709,8 +1987,17 @@
       <c r="G30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30">
+        <v>2022</v>
+      </c>
+      <c r="I30" t="s">
+        <v>207</v>
+      </c>
+      <c r="J30">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>123</v>
       </c>
@@ -1732,8 +2019,17 @@
       <c r="G31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31">
+        <v>2022</v>
+      </c>
+      <c r="I31" t="s">
+        <v>207</v>
+      </c>
+      <c r="J31" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>127</v>
       </c>
@@ -1755,8 +2051,17 @@
       <c r="G32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32">
+        <v>2022</v>
+      </c>
+      <c r="I32" t="s">
+        <v>207</v>
+      </c>
+      <c r="J32">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -1778,8 +2083,17 @@
       <c r="G33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33">
+        <v>2022</v>
+      </c>
+      <c r="I33" t="s">
+        <v>207</v>
+      </c>
+      <c r="J33">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -1801,8 +2115,17 @@
       <c r="G34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34">
+        <v>2022</v>
+      </c>
+      <c r="I34" t="s">
+        <v>207</v>
+      </c>
+      <c r="J34">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -1824,8 +2147,17 @@
       <c r="G35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35">
+        <v>2022</v>
+      </c>
+      <c r="I35" t="s">
+        <v>207</v>
+      </c>
+      <c r="J35">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -1847,8 +2179,17 @@
       <c r="G36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36">
+        <v>2022</v>
+      </c>
+      <c r="I36" t="s">
+        <v>207</v>
+      </c>
+      <c r="J36">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -1870,8 +2211,17 @@
       <c r="G37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37">
+        <v>2022</v>
+      </c>
+      <c r="I37" t="s">
+        <v>206</v>
+      </c>
+      <c r="J37">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -1893,8 +2243,17 @@
       <c r="G38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38">
+        <v>2022</v>
+      </c>
+      <c r="I38" t="s">
+        <v>206</v>
+      </c>
+      <c r="J38">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>155</v>
       </c>
@@ -1916,8 +2275,17 @@
       <c r="G39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39">
+        <v>2022</v>
+      </c>
+      <c r="I39" t="s">
+        <v>206</v>
+      </c>
+      <c r="J39">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>159</v>
       </c>
@@ -1939,8 +2307,17 @@
       <c r="G40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40">
+        <v>2022</v>
+      </c>
+      <c r="I40" t="s">
+        <v>206</v>
+      </c>
+      <c r="J40" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -1962,8 +2339,17 @@
       <c r="G41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41">
+        <v>2024</v>
+      </c>
+      <c r="I41" t="s">
+        <v>206</v>
+      </c>
+      <c r="J41">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -1985,8 +2371,17 @@
       <c r="G42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42">
+        <v>2024</v>
+      </c>
+      <c r="I42" t="s">
+        <v>206</v>
+      </c>
+      <c r="J42">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>171</v>
       </c>
@@ -2008,8 +2403,17 @@
       <c r="G43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43">
+        <v>2024</v>
+      </c>
+      <c r="I43" t="s">
+        <v>206</v>
+      </c>
+      <c r="J43" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>175</v>
       </c>
@@ -2031,8 +2435,17 @@
       <c r="G44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44">
+        <v>2024</v>
+      </c>
+      <c r="I44" t="s">
+        <v>206</v>
+      </c>
+      <c r="J44">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>179</v>
       </c>
@@ -2054,8 +2467,17 @@
       <c r="G45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45">
+        <v>2024</v>
+      </c>
+      <c r="I45" t="s">
+        <v>206</v>
+      </c>
+      <c r="J45">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>183</v>
       </c>
@@ -2077,8 +2499,17 @@
       <c r="G46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H46">
+        <v>2024</v>
+      </c>
+      <c r="I46" t="s">
+        <v>206</v>
+      </c>
+      <c r="J46">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>187</v>
       </c>
@@ -2100,8 +2531,17 @@
       <c r="G47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H47">
+        <v>2024</v>
+      </c>
+      <c r="I47" t="s">
+        <v>206</v>
+      </c>
+      <c r="J47">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>191</v>
       </c>
@@ -2123,8 +2563,17 @@
       <c r="G48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H48">
+        <v>2024</v>
+      </c>
+      <c r="I48" t="s">
+        <v>206</v>
+      </c>
+      <c r="J48">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>195</v>
       </c>
@@ -2146,8 +2595,17 @@
       <c r="G49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H49">
+        <v>2024</v>
+      </c>
+      <c r="I49" t="s">
+        <v>206</v>
+      </c>
+      <c r="J49">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>199</v>
       </c>
@@ -2168,6 +2626,15 @@
       </c>
       <c r="G50">
         <v>1</v>
+      </c>
+      <c r="H50">
+        <v>2024</v>
+      </c>
+      <c r="I50" t="s">
+        <v>206</v>
+      </c>
+      <c r="J50">
+        <v>3.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>